<commit_message>
update + growth rate reacceleration projection
</commit_message>
<xml_diff>
--- a/DDOG.xlsx
+++ b/DDOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffe\Documents\GitHub\martinshkreli-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B50DB-0A71-4894-B84A-351264157695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88AB9AE-FF4F-40BD-8881-5052BBAE5BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14235" yWindow="90" windowWidth="26190" windowHeight="20805" activeTab="1" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
+    <workbookView xWindow="14235" yWindow="90" windowWidth="37440" windowHeight="20805" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     Q2: 410-414m</t>
       </text>
     </comment>
-    <comment ref="V6" authorId="2" shapeId="0" xr:uid="{95169845-1F7F-4051-990A-FE3D69449576}">
+    <comment ref="Y6" authorId="2" shapeId="0" xr:uid="{95169845-1F7F-4051-990A-FE3D69449576}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     Q1: 1600-1620m</t>
       </text>
     </comment>
-    <comment ref="V7" authorId="3" shapeId="0" xr:uid="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
+    <comment ref="Y7" authorId="3" shapeId="0" xr:uid="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>Price</t>
   </si>
@@ -289,16 +289,36 @@
   </si>
   <si>
     <t>FY</t>
+  </si>
+  <si>
+    <t>Q323</t>
+  </si>
+  <si>
+    <t>YOY%</t>
+  </si>
+  <si>
+    <t>Q423</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>if growth accelerates up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -367,7 +387,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -406,6 +426,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -791,16 +816,16 @@
   <threadedComment ref="M6" dT="2022-09-02T14:59:12.36" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{15E8E758-37B6-468B-81A6-B3305FD6827A}">
     <text>Q2: 410-414m</text>
   </threadedComment>
-  <threadedComment ref="V6" dT="2022-09-02T14:59:40.61" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{95169845-1F7F-4051-990A-FE3D69449576}">
+  <threadedComment ref="Y6" dT="2022-09-02T14:59:40.61" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{95169845-1F7F-4051-990A-FE3D69449576}">
     <text>Q2: 1610-1630m</text>
   </threadedComment>
-  <threadedComment ref="V6" dT="2022-09-02T15:01:04.51" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{618BFB8A-809A-468A-BF3E-6286A5CBAEB3}" parentId="{95169845-1F7F-4051-990A-FE3D69449576}">
+  <threadedComment ref="Y6" dT="2022-09-02T15:01:04.51" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{618BFB8A-809A-468A-BF3E-6286A5CBAEB3}" parentId="{95169845-1F7F-4051-990A-FE3D69449576}">
     <text>Q1: 1600-1620m</text>
   </threadedComment>
-  <threadedComment ref="V7" dT="2022-09-02T14:59:40.61" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
+  <threadedComment ref="Y7" dT="2022-09-02T14:59:40.61" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
     <text>Q2: 1610-1630m</text>
   </threadedComment>
-  <threadedComment ref="V7" dT="2022-09-02T15:01:04.51" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{67F1968D-792E-4F6B-B86B-D7480C200BB9}" parentId="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
+  <threadedComment ref="Y7" dT="2022-09-02T15:01:04.51" personId="{6EBEE36F-B86D-4667-B671-D0667117F4FF}" id="{67F1968D-792E-4F6B-B86B-D7480C200BB9}" parentId="{939E2C75-C2A6-4046-AF27-AFF4D420F9BB}">
     <text>Q1: 1600-1620m</text>
   </threadedComment>
 </ThreadedComments>
@@ -810,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3BD0B1-E685-4627-8A01-75A3D2BDF860}">
   <dimension ref="N2:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -821,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>109.87</v>
+        <v>134.91</v>
       </c>
     </row>
     <row r="3" spans="14:16" x14ac:dyDescent="0.2">
@@ -829,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="5">
-        <v>296.27</v>
+        <v>325.55700000000002</v>
       </c>
       <c r="P3" s="2"/>
     </row>
@@ -839,7 +864,7 @@
       </c>
       <c r="O4" s="5">
         <f>+O2*O3</f>
-        <v>32551.1849</v>
+        <v>43920.894870000004</v>
       </c>
     </row>
     <row r="5" spans="14:16" x14ac:dyDescent="0.2">
@@ -847,7 +872,7 @@
         <v>3</v>
       </c>
       <c r="O5" s="5">
-        <v>2002</v>
+        <v>2080</v>
       </c>
       <c r="P5" s="2"/>
     </row>
@@ -856,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="O6" s="5">
-        <v>846.33</v>
+        <v>1736.826</v>
       </c>
       <c r="P6" s="2"/>
     </row>
@@ -866,7 +891,7 @@
       </c>
       <c r="O7" s="5">
         <f>+O4-O5+O6</f>
-        <v>31395.514900000002</v>
+        <v>43577.720870000005</v>
       </c>
     </row>
   </sheetData>
@@ -876,13 +901,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB5D0F6-F818-4D6B-9D91-E5CB5E0CBE0F}">
-  <dimension ref="A1:CZ54"/>
+  <dimension ref="A1:DC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
+      <selection pane="bottomRight" activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -891,11 +916,13 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="13" width="9.140625" style="2"/>
     <col min="14" max="14" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -911,11 +938,20 @@
       <c r="O1" s="14">
         <v>45016</v>
       </c>
-      <c r="S1" t="s">
+      <c r="P1" s="13">
+        <v>45107</v>
+      </c>
+      <c r="Q1" s="13">
+        <v>45199</v>
+      </c>
+      <c r="R1" s="13">
+        <v>45291</v>
+      </c>
+      <c r="V1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:104" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -958,50 +994,57 @@
       <c r="P2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2">
+      <c r="Q2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2">
         <v>2019</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>2020</v>
       </c>
-      <c r="U2">
-        <f>+T2+1</f>
+      <c r="X2">
+        <f>+W2+1</f>
         <v>2021</v>
       </c>
-      <c r="V2">
-        <f t="shared" ref="V2:X2" si="0">+U2+1</f>
+      <c r="Y2">
+        <f t="shared" ref="Y2:AA2" si="0">+X2+1</f>
         <v>2022</v>
       </c>
-      <c r="W2">
+      <c r="Z2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="Y2">
+      <c r="AB2">
         <v>2025</v>
       </c>
-      <c r="Z2">
+      <c r="AC2">
         <v>2026</v>
       </c>
-      <c r="AA2">
+      <c r="AD2">
         <v>2027</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>2028</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <v>2029</v>
       </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:104" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -1018,7 +1061,63 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="6" spans="1:104" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="Z4" s="25"/>
+    </row>
+    <row r="5" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="V5" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="22">
+        <f>(W6-V6)/V6</f>
+        <v>0.66344892221180896</v>
+      </c>
+      <c r="X5" s="22">
+        <f>(X6-W6)/W6</f>
+        <v>0.7047919849668417</v>
+      </c>
+      <c r="Y5" s="22">
+        <f>(Y6-X6)/X6</f>
+        <v>0.62823294296956378</v>
+      </c>
+      <c r="Z5" s="24">
+        <f>(Z6-Y6)/Y6</f>
+        <v>0.25783535311324701</v>
+      </c>
+      <c r="AA5" s="24">
+        <f>(AA6-Z6)/Z6</f>
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="AB5" s="24">
+        <f>(AB6-AA6)/AA6</f>
+        <v>0.26</v>
+      </c>
+      <c r="AC5" s="24">
+        <f>(AC6-AB6)/AB6</f>
+        <v>0.26000000000000012</v>
+      </c>
+      <c r="AD5" s="24">
+        <f>(AD6-AC6)/AC6</f>
+        <v>0.26</v>
+      </c>
+      <c r="AE5" s="24">
+        <f>(AE6-AD6)/AD6</f>
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="AF5" s="24">
+        <f>(AF6-AE6)/AE6</f>
+        <v>0.25999999999999995</v>
+      </c>
+      <c r="AG5" s="24">
+        <f>(AG6-AF6)/AF6</f>
+        <v>0.25999999999999995</v>
+      </c>
+      <c r="AH5" s="24">
+        <f>(AH6-AG6)/AG6</f>
+        <v>1.0000000000000038E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:107" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1060,349 +1159,354 @@
       <c r="P6" s="3">
         <v>509.64</v>
       </c>
-      <c r="S6" s="3">
+      <c r="Q6" s="3">
+        <v>547.53599999999994</v>
+      </c>
+      <c r="R6" s="3">
+        <v>568</v>
+      </c>
+      <c r="V6" s="3">
         <v>362.78</v>
       </c>
-      <c r="T6" s="3">
+      <c r="W6" s="3">
         <v>603.46600000000001</v>
       </c>
-      <c r="U6" s="3">
+      <c r="X6" s="3">
         <v>1028.7840000000001</v>
       </c>
-      <c r="V6" s="3">
+      <c r="Y6" s="3">
         <f>SUM($K$6:$N$6)</f>
         <v>1675.1</v>
       </c>
-      <c r="W6" s="3">
-        <f t="shared" ref="W6:AD6" si="1">V6*(1+$S$23)</f>
-        <v>2177.63</v>
-      </c>
-      <c r="X6" s="3">
-        <f t="shared" si="1"/>
-        <v>2830.9190000000003</v>
-      </c>
-      <c r="Y6" s="3">
-        <f t="shared" si="1"/>
-        <v>3680.1947000000005</v>
-      </c>
       <c r="Z6" s="3">
-        <f t="shared" si="1"/>
-        <v>4784.2531100000006</v>
+        <v>2107</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" si="1"/>
-        <v>6219.5290430000014</v>
+        <f t="shared" ref="Z6:AG7" si="1">Z6*(1+$V$23)</f>
+        <v>2654.82</v>
       </c>
       <c r="AB6" s="3">
         <f t="shared" si="1"/>
-        <v>8085.387755900002</v>
+        <v>3345.0732000000003</v>
       </c>
       <c r="AC6" s="3">
         <f t="shared" si="1"/>
-        <v>10511.004082670002</v>
+        <v>4214.7922320000007</v>
       </c>
       <c r="AD6" s="3">
         <f t="shared" si="1"/>
-        <v>13664.305307471004</v>
+        <v>5310.638212320001</v>
       </c>
       <c r="AE6" s="3">
-        <f>AD6*(1+S24)</f>
-        <v>13800.948360545714</v>
+        <f t="shared" si="1"/>
+        <v>6691.4041475232016</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" ref="AF6:CQ6" si="2">AE6*(1+T24)</f>
-        <v>13800.948360545714</v>
+        <f t="shared" si="1"/>
+        <v>8431.1692258792336</v>
       </c>
       <c r="AG6" s="3">
-        <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <f t="shared" si="1"/>
+        <v>10623.273224607834</v>
       </c>
       <c r="AH6" s="3">
-        <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <f>AG6*(1+$V$24)</f>
+        <v>10729.505956853913</v>
       </c>
       <c r="AI6" s="3">
-        <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <f t="shared" ref="AI6:CT6" si="2">AH6*(1+$V$24)</f>
+        <v>10836.801016422452</v>
       </c>
       <c r="AJ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>10945.169026586676</v>
       </c>
       <c r="AK6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11054.620716852543</v>
       </c>
       <c r="AL6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11165.166924021069</v>
       </c>
       <c r="AM6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11276.81859326128</v>
       </c>
       <c r="AN6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11389.586779193893</v>
       </c>
       <c r="AO6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11503.482646985831</v>
       </c>
       <c r="AP6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11618.517473455689</v>
       </c>
       <c r="AQ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11734.702648190247</v>
       </c>
       <c r="AR6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11852.049674672149</v>
       </c>
       <c r="AS6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>11970.570171418871</v>
       </c>
       <c r="AT6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12090.27587313306</v>
       </c>
       <c r="AU6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12211.17863186439</v>
       </c>
       <c r="AV6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12333.290418183034</v>
       </c>
       <c r="AW6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12456.623322364865</v>
       </c>
       <c r="AX6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12581.189555588513</v>
       </c>
       <c r="AY6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12707.001451144399</v>
       </c>
       <c r="AZ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12834.071465655843</v>
       </c>
       <c r="BA6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>12962.412180312402</v>
       </c>
       <c r="BB6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13092.036302115526</v>
       </c>
       <c r="BC6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13222.956665136682</v>
       </c>
       <c r="BD6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13355.18623178805</v>
       </c>
       <c r="BE6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13488.738094105931</v>
       </c>
       <c r="BF6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13623.625475046991</v>
       </c>
       <c r="BG6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13759.861729797462</v>
       </c>
       <c r="BH6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>13897.460347095437</v>
       </c>
       <c r="BI6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14036.434950566392</v>
       </c>
       <c r="BJ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14176.799300072056</v>
       </c>
       <c r="BK6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14318.567293072776</v>
       </c>
       <c r="BL6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14461.752966003503</v>
       </c>
       <c r="BM6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14606.370495663539</v>
       </c>
       <c r="BN6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14752.434200620175</v>
       </c>
       <c r="BO6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>14899.958542626377</v>
       </c>
       <c r="BP6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15048.95812805264</v>
       </c>
       <c r="BQ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15199.447709333166</v>
       </c>
       <c r="BR6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15351.442186426499</v>
       </c>
       <c r="BS6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15504.956608290764</v>
       </c>
       <c r="BT6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15660.006174373671</v>
       </c>
       <c r="BU6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15816.606236117408</v>
       </c>
       <c r="BV6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>15974.772298478581</v>
       </c>
       <c r="BW6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16134.520021463368</v>
       </c>
       <c r="BX6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16295.865221678001</v>
       </c>
       <c r="BY6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16458.82387389478</v>
       </c>
       <c r="BZ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16623.412112633727</v>
       </c>
       <c r="CA6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16789.646233760064</v>
       </c>
       <c r="CB6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>16957.542696097666</v>
       </c>
       <c r="CC6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>17127.118123058641</v>
       </c>
       <c r="CD6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>17298.389304289227</v>
       </c>
       <c r="CE6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>17471.373197332119</v>
       </c>
       <c r="CF6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>17646.086929305442</v>
       </c>
       <c r="CG6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>17822.547798598498</v>
       </c>
       <c r="CH6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18000.773276584485</v>
       </c>
       <c r="CI6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18180.781009350329</v>
       </c>
       <c r="CJ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18362.58881944383</v>
       </c>
       <c r="CK6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18546.214707638268</v>
       </c>
       <c r="CL6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18731.676854714649</v>
       </c>
       <c r="CM6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>18918.993623261795</v>
       </c>
       <c r="CN6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>19108.183559494413</v>
       </c>
       <c r="CO6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>19299.265395089358</v>
       </c>
       <c r="CP6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>19492.258049040251</v>
       </c>
       <c r="CQ6" s="3">
         <f t="shared" si="2"/>
-        <v>13800.948360545714</v>
+        <v>19687.180629530652</v>
       </c>
       <c r="CR6" s="3">
-        <f t="shared" ref="CR6:CZ6" si="3">CQ6*(1+CF24)</f>
-        <v>13800.948360545714</v>
+        <f t="shared" si="2"/>
+        <v>19884.052435825961</v>
       </c>
       <c r="CS6" s="3">
-        <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <f t="shared" si="2"/>
+        <v>20082.892960184221</v>
       </c>
       <c r="CT6" s="3">
-        <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <f t="shared" si="2"/>
+        <v>20283.721889786062</v>
       </c>
       <c r="CU6" s="3">
-        <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <f t="shared" ref="CU6:DC6" si="3">CT6*(1+$V$24)</f>
+        <v>20486.559108683923</v>
       </c>
       <c r="CV6" s="3">
         <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <v>20691.424699770763</v>
       </c>
       <c r="CW6" s="3">
         <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <v>20898.338946768472</v>
       </c>
       <c r="CX6" s="3">
         <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <v>21107.322336236157</v>
       </c>
       <c r="CY6" s="3">
         <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
+        <v>21318.395559598517</v>
       </c>
       <c r="CZ6" s="3">
         <f t="shared" si="3"/>
-        <v>13800.948360545714</v>
-      </c>
-    </row>
-    <row r="7" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>21531.579515194502</v>
+      </c>
+      <c r="DA6" s="3">
+        <f t="shared" si="3"/>
+        <v>21746.895310346448</v>
+      </c>
+      <c r="DB6" s="3">
+        <f t="shared" si="3"/>
+        <v>21964.364263449912</v>
+      </c>
+      <c r="DC6" s="3">
+        <f t="shared" si="3"/>
+        <v>22184.007906084411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1444,80 +1548,447 @@
       <c r="P7" s="5">
         <v>101.846</v>
       </c>
-      <c r="S7" s="3">
+      <c r="Q7" s="5">
+        <v>103.319</v>
+      </c>
+      <c r="V7" s="3">
         <v>362.78</v>
       </c>
-      <c r="T7" s="3">
+      <c r="W7" s="3">
         <v>603.46600000000001</v>
       </c>
-      <c r="U7" s="3">
+      <c r="X7" s="3">
         <v>1028.7840000000001</v>
       </c>
-      <c r="V7" s="3">
+      <c r="Y7" s="3">
         <f>SUM($K$6:$N$6)</f>
         <v>1675.1</v>
       </c>
-      <c r="W7" s="5">
-        <f>SUM(O6:R6)</f>
-        <v>991.35400000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z7" s="5">
+        <f>SUM(O6:U6)</f>
+        <v>2106.89</v>
+      </c>
+      <c r="AA7" s="3">
+        <f>Z7*(1+$X$23)</f>
+        <v>2738.9569999999999</v>
+      </c>
+      <c r="AB7" s="3">
+        <f>AA7*(1+$X$23)</f>
+        <v>3560.6441</v>
+      </c>
+      <c r="AC7" s="3">
+        <f>AB7*(1+$X$23)</f>
+        <v>4628.8373300000003</v>
+      </c>
+      <c r="AD7" s="3">
+        <f>AC7*(1+$X$23)</f>
+        <v>6017.4885290000002</v>
+      </c>
+      <c r="AE7" s="3">
+        <f>AD7*(1+$X$23)</f>
+        <v>7822.7350877000008</v>
+      </c>
+      <c r="AF7" s="3">
+        <f>AE7*(1+$X$23)</f>
+        <v>10169.555614010002</v>
+      </c>
+      <c r="AG7" s="3">
+        <f>AF7*(1+$X$23)</f>
+        <v>13220.422298213003</v>
+      </c>
+      <c r="AH7" s="3">
+        <f>AG7*(1+$V$24)</f>
+        <v>13352.626521195134</v>
+      </c>
+      <c r="AI7" s="3">
+        <f>AH7*(1+$V$24)</f>
+        <v>13486.152786407085</v>
+      </c>
+      <c r="AJ7" s="3">
+        <f t="shared" ref="AJ7:CU7" si="4">AI7*(1+$V$24)</f>
+        <v>13621.014314271157</v>
+      </c>
+      <c r="AK7" s="3">
+        <f t="shared" si="4"/>
+        <v>13757.224457413868</v>
+      </c>
+      <c r="AL7" s="3">
+        <f t="shared" si="4"/>
+        <v>13894.796701988007</v>
+      </c>
+      <c r="AM7" s="3">
+        <f t="shared" si="4"/>
+        <v>14033.744669007887</v>
+      </c>
+      <c r="AN7" s="3">
+        <f t="shared" si="4"/>
+        <v>14174.082115697965</v>
+      </c>
+      <c r="AO7" s="3">
+        <f t="shared" si="4"/>
+        <v>14315.822936854946</v>
+      </c>
+      <c r="AP7" s="3">
+        <f t="shared" si="4"/>
+        <v>14458.981166223495</v>
+      </c>
+      <c r="AQ7" s="3">
+        <f t="shared" si="4"/>
+        <v>14603.570977885731</v>
+      </c>
+      <c r="AR7" s="3">
+        <f t="shared" si="4"/>
+        <v>14749.606687664589</v>
+      </c>
+      <c r="AS7" s="3">
+        <f t="shared" si="4"/>
+        <v>14897.102754541234</v>
+      </c>
+      <c r="AT7" s="3">
+        <f t="shared" si="4"/>
+        <v>15046.073782086647</v>
+      </c>
+      <c r="AU7" s="3">
+        <f t="shared" si="4"/>
+        <v>15196.534519907515</v>
+      </c>
+      <c r="AV7" s="3">
+        <f t="shared" si="4"/>
+        <v>15348.499865106591</v>
+      </c>
+      <c r="AW7" s="3">
+        <f t="shared" si="4"/>
+        <v>15501.984863757656</v>
+      </c>
+      <c r="AX7" s="3">
+        <f t="shared" si="4"/>
+        <v>15657.004712395234</v>
+      </c>
+      <c r="AY7" s="3">
+        <f t="shared" si="4"/>
+        <v>15813.574759519186</v>
+      </c>
+      <c r="AZ7" s="3">
+        <f t="shared" si="4"/>
+        <v>15971.710507114378</v>
+      </c>
+      <c r="BA7" s="3">
+        <f t="shared" si="4"/>
+        <v>16131.427612185522</v>
+      </c>
+      <c r="BB7" s="3">
+        <f t="shared" si="4"/>
+        <v>16292.741888307377</v>
+      </c>
+      <c r="BC7" s="3">
+        <f t="shared" si="4"/>
+        <v>16455.669307190452</v>
+      </c>
+      <c r="BD7" s="3">
+        <f t="shared" si="4"/>
+        <v>16620.226000262355</v>
+      </c>
+      <c r="BE7" s="3">
+        <f t="shared" si="4"/>
+        <v>16786.42826026498</v>
+      </c>
+      <c r="BF7" s="3">
+        <f t="shared" si="4"/>
+        <v>16954.292542867632</v>
+      </c>
+      <c r="BG7" s="3">
+        <f t="shared" si="4"/>
+        <v>17123.835468296307</v>
+      </c>
+      <c r="BH7" s="3">
+        <f t="shared" si="4"/>
+        <v>17295.07382297927</v>
+      </c>
+      <c r="BI7" s="3">
+        <f t="shared" si="4"/>
+        <v>17468.024561209062</v>
+      </c>
+      <c r="BJ7" s="3">
+        <f t="shared" si="4"/>
+        <v>17642.704806821152</v>
+      </c>
+      <c r="BK7" s="3">
+        <f t="shared" si="4"/>
+        <v>17819.131854889365</v>
+      </c>
+      <c r="BL7" s="3">
+        <f t="shared" si="4"/>
+        <v>17997.323173438257</v>
+      </c>
+      <c r="BM7" s="3">
+        <f t="shared" si="4"/>
+        <v>18177.296405172641</v>
+      </c>
+      <c r="BN7" s="3">
+        <f t="shared" si="4"/>
+        <v>18359.069369224369</v>
+      </c>
+      <c r="BO7" s="3">
+        <f t="shared" si="4"/>
+        <v>18542.660062916613</v>
+      </c>
+      <c r="BP7" s="3">
+        <f t="shared" si="4"/>
+        <v>18728.086663545779</v>
+      </c>
+      <c r="BQ7" s="3">
+        <f t="shared" si="4"/>
+        <v>18915.367530181236</v>
+      </c>
+      <c r="BR7" s="3">
+        <f t="shared" si="4"/>
+        <v>19104.521205483048</v>
+      </c>
+      <c r="BS7" s="3">
+        <f t="shared" si="4"/>
+        <v>19295.566417537877</v>
+      </c>
+      <c r="BT7" s="3">
+        <f t="shared" si="4"/>
+        <v>19488.522081713258</v>
+      </c>
+      <c r="BU7" s="3">
+        <f t="shared" si="4"/>
+        <v>19683.407302530391</v>
+      </c>
+      <c r="BV7" s="3">
+        <f t="shared" si="4"/>
+        <v>19880.241375555695</v>
+      </c>
+      <c r="BW7" s="3">
+        <f t="shared" si="4"/>
+        <v>20079.043789311254</v>
+      </c>
+      <c r="BX7" s="3">
+        <f t="shared" si="4"/>
+        <v>20279.834227204366</v>
+      </c>
+      <c r="BY7" s="3">
+        <f t="shared" si="4"/>
+        <v>20482.632569476409</v>
+      </c>
+      <c r="BZ7" s="3">
+        <f t="shared" si="4"/>
+        <v>20687.458895171174</v>
+      </c>
+      <c r="CA7" s="3">
+        <f t="shared" si="4"/>
+        <v>20894.333484122886</v>
+      </c>
+      <c r="CB7" s="3">
+        <f t="shared" si="4"/>
+        <v>21103.276818964114</v>
+      </c>
+      <c r="CC7" s="3">
+        <f t="shared" si="4"/>
+        <v>21314.309587153755</v>
+      </c>
+      <c r="CD7" s="3">
+        <f t="shared" si="4"/>
+        <v>21527.452683025294</v>
+      </c>
+      <c r="CE7" s="3">
+        <f t="shared" si="4"/>
+        <v>21742.727209855548</v>
+      </c>
+      <c r="CF7" s="3">
+        <f t="shared" si="4"/>
+        <v>21960.154481954105</v>
+      </c>
+      <c r="CG7" s="3">
+        <f t="shared" si="4"/>
+        <v>22179.756026773648</v>
+      </c>
+      <c r="CH7" s="3">
+        <f t="shared" si="4"/>
+        <v>22401.553587041384</v>
+      </c>
+      <c r="CI7" s="3">
+        <f t="shared" si="4"/>
+        <v>22625.569122911798</v>
+      </c>
+      <c r="CJ7" s="3">
+        <f t="shared" si="4"/>
+        <v>22851.824814140917</v>
+      </c>
+      <c r="CK7" s="3">
+        <f t="shared" si="4"/>
+        <v>23080.343062282325</v>
+      </c>
+      <c r="CL7" s="3">
+        <f t="shared" si="4"/>
+        <v>23311.146492905147</v>
+      </c>
+      <c r="CM7" s="3">
+        <f t="shared" si="4"/>
+        <v>23544.257957834197</v>
+      </c>
+      <c r="CN7" s="3">
+        <f t="shared" si="4"/>
+        <v>23779.70053741254</v>
+      </c>
+      <c r="CO7" s="3">
+        <f t="shared" si="4"/>
+        <v>24017.497542786667</v>
+      </c>
+      <c r="CP7" s="3">
+        <f t="shared" si="4"/>
+        <v>24257.672518214535</v>
+      </c>
+      <c r="CQ7" s="3">
+        <f t="shared" si="4"/>
+        <v>24500.24924339668</v>
+      </c>
+      <c r="CR7" s="3">
+        <f t="shared" si="4"/>
+        <v>24745.251735830647</v>
+      </c>
+      <c r="CS7" s="3">
+        <f t="shared" si="4"/>
+        <v>24992.704253188953</v>
+      </c>
+      <c r="CT7" s="3">
+        <f t="shared" si="4"/>
+        <v>25242.631295720843</v>
+      </c>
+      <c r="CU7" s="3">
+        <f t="shared" si="4"/>
+        <v>25495.057608678053</v>
+      </c>
+      <c r="CV7" s="3">
+        <f t="shared" ref="CV7:DC7" si="5">CU7*(1+$V$24)</f>
+        <v>25750.008184764833</v>
+      </c>
+      <c r="CW7" s="3">
+        <f t="shared" si="5"/>
+        <v>26007.50826661248</v>
+      </c>
+      <c r="CX7" s="3">
+        <f t="shared" si="5"/>
+        <v>26267.583349278604</v>
+      </c>
+      <c r="CY7" s="3">
+        <f t="shared" si="5"/>
+        <v>26530.259182771391</v>
+      </c>
+      <c r="CZ7" s="3">
+        <f t="shared" si="5"/>
+        <v>26795.561774599104</v>
+      </c>
+      <c r="DA7" s="3">
+        <f t="shared" si="5"/>
+        <v>27063.517392345097</v>
+      </c>
+      <c r="DB7" s="3">
+        <f t="shared" si="5"/>
+        <v>27334.152566268549</v>
+      </c>
+      <c r="DC7" s="3">
+        <f t="shared" si="5"/>
+        <v>27607.494091931236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
-        <f t="shared" ref="E8:P8" si="4">+E6-E7</f>
+        <f t="shared" ref="E8:Q8" si="6">+E6-E7</f>
         <v>120.691</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>136.67500000000001</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>151.88300000000001</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>176.45100000000002</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>207.15600000000001</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>259.04899999999998</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>288.56799999999998</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>324.21299999999997</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>342.93400000000003</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>372.642</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>381.8</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>407.79399999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q8" s="6">
+        <f t="shared" si="6"/>
+        <v>444.21699999999993</v>
+      </c>
+      <c r="Z8" s="24">
+        <f>(Z7-Y7)/Y7</f>
+        <v>0.25776968539191691</v>
+      </c>
+      <c r="AA8" s="22">
+        <f>(AA7-Z7)/Z7</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AB8" s="22">
+        <f>(AB7-AA7)/AA7</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AC8" s="22">
+        <f>(AC7-AB7)/AB7</f>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="AD8" s="22">
+        <f>(AD7-AC7)/AC7</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="AE8" s="22">
+        <f>(AE7-AD7)/AD7</f>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="AF8" s="22">
+        <f>(AF7-AE7)/AE7</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AG8" s="22">
+        <f>(AG7-AF7)/AF7</f>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="AH8" s="22">
+        <f>(AH7-AG7)/AG7</f>
+        <v>1.0000000000000064E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1559,8 +2030,11 @@
       <c r="P9" s="5">
         <v>239.494</v>
       </c>
-    </row>
-    <row r="10" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q9" s="5">
+        <v>240.22499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1602,8 +2076,11 @@
       <c r="P10" s="5">
         <v>147.45500000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5">
+        <v>156.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1645,94 +2122,101 @@
       <c r="P11" s="5">
         <v>42.670999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q11" s="5">
+        <v>51.351999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
-        <f t="shared" ref="E12:P12" si="5">SUM(E9:E11)</f>
+        <f t="shared" ref="E12:Q12" si="7">SUM(E9:E11)</f>
         <v>129.958</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>145.613</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>164.71299999999999</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>186.33699999999999</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212.05100000000002</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>250.59399999999999</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>278.154</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>327.35199999999998</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>374.27599999999995</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>407.27</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>416.77</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>429.62</v>
       </c>
-    </row>
-    <row r="13" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q12" s="6">
+        <f t="shared" si="7"/>
+        <v>448.447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
-        <f t="shared" ref="E13:P13" si="6">E8-E12</f>
+        <f t="shared" ref="E13:Q13" si="8">E8-E12</f>
         <v>-9.2669999999999959</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-8.9379999999999882</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-12.829999999999984</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-9.8859999999999673</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-4.8950000000000102</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.4549999999999841</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10.413999999999987</v>
       </c>
       <c r="L13" s="6">
@@ -1740,23 +2224,27 @@
         <v>-3.13900000000001</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-31.341999999999928</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-34.627999999999986</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-34.96999999999997</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-21.826000000000022</v>
       </c>
-    </row>
-    <row r="14" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q13" s="6">
+        <f t="shared" si="8"/>
+        <v>-4.230000000000075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1807,63 +2295,71 @@
         <f>22.624-1.526</f>
         <v>21.097999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q14" s="5">
+        <f>-1.303+29.883</f>
+        <v>28.58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
-        <f t="shared" ref="E15:P15" si="7">+E13+E14</f>
+        <f t="shared" ref="E15:Q15" si="9">+E13+E14</f>
         <v>-14.554999999999996</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-15.166999999999987</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-12.528999999999986</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-9.6579999999999675</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-4.7670000000000101</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8.531999999999984</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>10.853999999999989</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-1.1000000000010779E-2</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-22.21599999999993</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-25.009999999999987</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-20.423999999999971</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.72800000000002285</v>
       </c>
-    </row>
-    <row r="16" spans="1:104" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q15" s="6">
+        <f t="shared" si="9"/>
+        <v>24.349999999999923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
@@ -1905,118 +2401,129 @@
       <c r="P16" s="5">
         <v>3.0609999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q16" s="5">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
-        <f t="shared" ref="E17:P17" si="8">+E15-E16</f>
+        <f t="shared" ref="E17:Q17" si="10">+E15-E16</f>
         <v>-15.149999999999997</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-16.159999999999986</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-11.989999999999986</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-6.6979999999999675</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.0500000000000105</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.1689999999999845</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.7379999999999889</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.8790000000000111</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-25.141999999999932</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-28.189999999999987</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-24.08599999999997</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.7890000000000228</v>
       </c>
-    </row>
-    <row r="18" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q17" s="6">
+        <f t="shared" si="10"/>
+        <v>22.679999999999922</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7">
-        <f t="shared" ref="E18:P18" si="9">+E17/E19</f>
+        <f t="shared" ref="E18:Q18" si="11">+E17/E19</f>
         <v>-5.0073705850856368E-2</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-5.3147929500060795E-2</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-3.9178653352241861E-2</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-2.1745411809011676E-2</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.3054114947122809E-2</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.0727021455604115E-2</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.8171540321927365E-2</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.5498975523753589E-2</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-7.9565809044589805E-2</v>
       </c>
       <c r="N18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-8.8829928028536453E-2</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-7.5437068960117162E-2</v>
       </c>
       <c r="P18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.1759229086169245E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q18" s="7">
+        <f t="shared" si="11"/>
+        <v>6.9665219915406279E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
@@ -2058,8 +2565,11 @@
       <c r="P19" s="5">
         <v>322.21499999999997</v>
       </c>
-    </row>
-    <row r="21" spans="2:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q19" s="5">
+        <v>325.55700000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
@@ -2070,15 +2580,15 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10">
-        <f t="shared" ref="I21:K21" si="10">+I6/E6-1</f>
+        <f t="shared" ref="I21:K21" si="12">+I6/E6-1</f>
         <v>0.74875060610958455</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.83741431074009598</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.82841515192723181</v>
       </c>
       <c r="L21" s="10">
@@ -2101,37 +2611,45 @@
         <f>+P6/L6-1</f>
         <v>0.25484441249033574</v>
       </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q21" s="10">
+        <f>+Q6/M6-1</f>
+        <v>0.25428318134024219</v>
+      </c>
+      <c r="R21" s="10">
+        <f>+R6/N6-1</f>
+        <v>0.21005796774172936</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E22" s="12">
-        <f t="shared" ref="E22:H22" si="11">+E8/E6</f>
+        <f t="shared" ref="E22:H22" si="13">+E8/E6</f>
         <v>0.78028770001616288</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.76986554460911061</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.7649648197674126</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.75552025485015994</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:K22" si="12">+I8/I6</f>
+        <f t="shared" ref="I22:K22" si="14">+I8/I6</f>
         <v>0.76586022300434775</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.79414649997854059</v>
       </c>
       <c r="K22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.79488747486433631</v>
       </c>
       <c r="L22" s="12">
@@ -2139,31 +2657,50 @@
         <v>0.79828284967178642</v>
       </c>
       <c r="M22" s="12">
-        <f t="shared" ref="M22:P22" si="13">+M8/M6</f>
+        <f t="shared" ref="M22:Q22" si="15">+M8/M6</f>
         <v>0.78558551129009724</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.79387045988593929</v>
       </c>
       <c r="O22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.79258647247121738</v>
       </c>
       <c r="P22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.8001608978887057</v>
       </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="R23" s="15" t="s">
+      <c r="Q22" s="12">
+        <f t="shared" si="15"/>
+        <v>0.81130190526285029</v>
+      </c>
+      <c r="U22" t="s">
+        <v>71</v>
+      </c>
+      <c r="W22" t="s">
+        <v>72</v>
+      </c>
+      <c r="X22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="U23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="S23" s="20">
+      <c r="V23" s="23">
+        <v>0.26</v>
+      </c>
+      <c r="W23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="X23" s="23">
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
@@ -2185,14 +2722,14 @@
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-      <c r="R24" s="17" t="s">
+      <c r="U24" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="S24" s="16">
+      <c r="V24" s="16">
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
@@ -2212,14 +2749,14 @@
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="R25" s="17" t="s">
+      <c r="U25" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="S25" s="16">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V25" s="16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
@@ -2241,15 +2778,22 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="R26" s="17" t="s">
+      <c r="U26" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="S26" s="18">
-        <f>NPV(S25,S6:CZ6)</f>
-        <v>57693.064395439622</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V26" s="18">
+        <f>NPV(V25,V6:DC6)</f>
+        <v>58324.781680299697</v>
+      </c>
+      <c r="W26" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="X26" s="26">
+        <f>NPV($V$25,V7:DC7)</f>
+        <v>70118.732659662914</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
@@ -2269,15 +2813,22 @@
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
-      <c r="R27" s="17" t="s">
+      <c r="U27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="S27" s="21">
-        <f>Main!O3</f>
-        <v>296.27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V27" s="21">
+        <f>Main!$O$3</f>
+        <v>325.55700000000002</v>
+      </c>
+      <c r="W27" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="X27" s="21">
+        <f>Main!$O$3</f>
+        <v>325.55700000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
@@ -2297,15 +2848,22 @@
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="R28" s="17" t="s">
+      <c r="U28" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="S28" s="19">
-        <f>S26/S27</f>
-        <v>194.73137474411729</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V28" s="19">
+        <f>V26/V27</f>
+        <v>179.1538246153506</v>
+      </c>
+      <c r="W28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="X28" s="19">
+        <f>X26/X27</f>
+        <v>215.38081706018579</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>37</v>
       </c>
@@ -2325,15 +2883,22 @@
       </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="R29" s="17" t="s">
+      <c r="U29" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="S29" s="20">
-        <f>(S28-Main!O2)/Main!O2</f>
-        <v>0.77237985568505763</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V29" s="20">
+        <f>(V28-Main!$O$2)/Main!$O$2</f>
+        <v>0.32795066796642652</v>
+      </c>
+      <c r="W29" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="X29" s="20">
+        <f>(X28-Main!$O$2)/Main!$O$2</f>
+        <v>0.59647777822389592</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>38</v>
       </c>
@@ -2355,15 +2920,22 @@
       </c>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-      <c r="R30" s="17" t="s">
+      <c r="U30" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="S30" s="18">
-        <f>S27*S28</f>
-        <v>57693.064395439629</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V30" s="18">
+        <f>V27*V28</f>
+        <v>58324.781680299697</v>
+      </c>
+      <c r="W30" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="X30" s="18">
+        <f>X27*X28</f>
+        <v>70118.732659662914</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2384,7 +2956,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="2:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
update with q423 results
</commit_message>
<xml_diff>
--- a/DDOG.xlsx
+++ b/DDOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffe\Documents\GitHub\martinshkreli-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88AB9AE-FF4F-40BD-8881-5052BBAE5BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A787C9-DEDB-49DF-98D5-D831FFAE8E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14235" yWindow="90" windowWidth="37440" windowHeight="20805" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Price</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>if growth accelerates up</t>
+  </si>
+  <si>
+    <t>Q124</t>
   </si>
 </sst>
 </file>
@@ -835,39 +838,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3BD0B1-E685-4627-8A01-75A3D2BDF860}">
   <dimension ref="N2:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N2" t="s">
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>134.91</v>
-      </c>
-    </row>
-    <row r="3" spans="14:16" x14ac:dyDescent="0.2">
+        <v>129.74</v>
+      </c>
+    </row>
+    <row r="3" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N3" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="5">
-        <v>325.55700000000002</v>
+        <v>328</v>
       </c>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N4" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="5">
         <f>+O2*O3</f>
-        <v>43920.894870000004</v>
-      </c>
-    </row>
-    <row r="5" spans="14:16" x14ac:dyDescent="0.2">
+        <v>42554.720000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N5" t="s">
         <v>3</v>
       </c>
@@ -876,7 +879,7 @@
       </c>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N6" t="s">
         <v>4</v>
       </c>
@@ -885,13 +888,13 @@
       </c>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N7" t="s">
         <v>5</v>
       </c>
       <c r="O7" s="5">
         <f>+O4-O5+O6</f>
-        <v>43577.720870000005</v>
+        <v>42211.546000000002</v>
       </c>
     </row>
   </sheetData>
@@ -903,26 +906,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB5D0F6-F818-4D6B-9D91-E5CB5E0CBE0F}">
   <dimension ref="A1:DC54"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X23" sqref="X23"/>
+      <selection pane="bottomRight" activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="13" width="9.109375" style="2"/>
+    <col min="14" max="14" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -947,11 +951,14 @@
       <c r="R1" s="13">
         <v>45291</v>
       </c>
+      <c r="S1" s="14">
+        <v>45382</v>
+      </c>
       <c r="V1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +1007,9 @@
       <c r="R2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2">
@@ -1044,7 +1053,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -1061,63 +1070,63 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
       <c r="Z4" s="25"/>
     </row>
-    <row r="5" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:107" x14ac:dyDescent="0.25">
       <c r="V5" t="s">
         <v>69</v>
       </c>
       <c r="W5" s="22">
-        <f>(W6-V6)/V6</f>
+        <f t="shared" ref="W5:AH5" si="1">(W6-V6)/V6</f>
         <v>0.66344892221180896</v>
       </c>
       <c r="X5" s="22">
-        <f>(X6-W6)/W6</f>
+        <f t="shared" si="1"/>
         <v>0.7047919849668417</v>
       </c>
       <c r="Y5" s="22">
-        <f>(Y6-X6)/X6</f>
+        <f t="shared" si="1"/>
         <v>0.62823294296956378</v>
       </c>
       <c r="Z5" s="24">
-        <f>(Z6-Y6)/Y6</f>
+        <f t="shared" si="1"/>
         <v>0.25783535311324701</v>
       </c>
       <c r="AA5" s="24">
         <f>(AA6-Z6)/Z6</f>
-        <v>0.26000000000000006</v>
+        <v>0.23999999999999994</v>
       </c>
       <c r="AB5" s="24">
-        <f>(AB6-AA6)/AA6</f>
-        <v>0.26</v>
+        <f t="shared" si="1"/>
+        <v>0.24000000000000005</v>
       </c>
       <c r="AC5" s="24">
-        <f>(AC6-AB6)/AB6</f>
-        <v>0.26000000000000012</v>
+        <f t="shared" si="1"/>
+        <v>0.23999999999999996</v>
       </c>
       <c r="AD5" s="24">
-        <f>(AD6-AC6)/AC6</f>
-        <v>0.26</v>
+        <f t="shared" si="1"/>
+        <v>0.23999999999999994</v>
       </c>
       <c r="AE5" s="24">
-        <f>(AE6-AD6)/AD6</f>
-        <v>0.26000000000000006</v>
+        <f t="shared" si="1"/>
+        <v>0.24000000000000002</v>
       </c>
       <c r="AF5" s="24">
-        <f>(AF6-AE6)/AE6</f>
-        <v>0.25999999999999995</v>
+        <f t="shared" si="1"/>
+        <v>0.23999999999999994</v>
       </c>
       <c r="AG5" s="24">
-        <f>(AG6-AF6)/AF6</f>
-        <v>0.25999999999999995</v>
+        <f t="shared" si="1"/>
+        <v>0.23999999999999994</v>
       </c>
       <c r="AH5" s="24">
-        <f>(AH6-AG6)/AG6</f>
-        <v>1.0000000000000038E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:107" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000097E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:107" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1172,11 @@
         <v>547.53599999999994</v>
       </c>
       <c r="R6" s="3">
-        <v>568</v>
+        <v>589.649</v>
+      </c>
+      <c r="S6" s="3">
+        <f>(587+591)/2</f>
+        <v>589</v>
       </c>
       <c r="V6" s="3">
         <v>362.78</v>
@@ -1182,331 +1195,331 @@
         <v>2107</v>
       </c>
       <c r="AA6" s="3">
-        <f t="shared" ref="Z6:AG7" si="1">Z6*(1+$V$23)</f>
-        <v>2654.82</v>
+        <f t="shared" ref="AA6:AG6" si="2">Z6*(1+$V$23)</f>
+        <v>2612.6799999999998</v>
       </c>
       <c r="AB6" s="3">
-        <f t="shared" si="1"/>
-        <v>3345.0732000000003</v>
+        <f t="shared" si="2"/>
+        <v>3239.7231999999999</v>
       </c>
       <c r="AC6" s="3">
-        <f t="shared" si="1"/>
-        <v>4214.7922320000007</v>
+        <f t="shared" si="2"/>
+        <v>4017.2567679999997</v>
       </c>
       <c r="AD6" s="3">
-        <f t="shared" si="1"/>
-        <v>5310.638212320001</v>
+        <f t="shared" si="2"/>
+        <v>4981.3983923199994</v>
       </c>
       <c r="AE6" s="3">
-        <f t="shared" si="1"/>
-        <v>6691.4041475232016</v>
+        <f t="shared" si="2"/>
+        <v>6176.9340064767994</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" si="1"/>
-        <v>8431.1692258792336</v>
+        <f t="shared" si="2"/>
+        <v>7659.3981680312309</v>
       </c>
       <c r="AG6" s="3">
-        <f t="shared" si="1"/>
-        <v>10623.273224607834</v>
+        <f t="shared" si="2"/>
+        <v>9497.6537283587259</v>
       </c>
       <c r="AH6" s="3">
         <f>AG6*(1+$V$24)</f>
-        <v>10729.505956853913</v>
+        <v>9592.630265642314</v>
       </c>
       <c r="AI6" s="3">
-        <f t="shared" ref="AI6:CT6" si="2">AH6*(1+$V$24)</f>
-        <v>10836.801016422452</v>
+        <f t="shared" ref="AI6:CT6" si="3">AH6*(1+$V$24)</f>
+        <v>9688.5565682987381</v>
       </c>
       <c r="AJ6" s="3">
-        <f t="shared" si="2"/>
-        <v>10945.169026586676</v>
+        <f t="shared" si="3"/>
+        <v>9785.4421339817254</v>
       </c>
       <c r="AK6" s="3">
-        <f t="shared" si="2"/>
-        <v>11054.620716852543</v>
+        <f t="shared" si="3"/>
+        <v>9883.2965553215436</v>
       </c>
       <c r="AL6" s="3">
-        <f t="shared" si="2"/>
-        <v>11165.166924021069</v>
+        <f t="shared" si="3"/>
+        <v>9982.1295208747597</v>
       </c>
       <c r="AM6" s="3">
-        <f t="shared" si="2"/>
-        <v>11276.81859326128</v>
+        <f t="shared" si="3"/>
+        <v>10081.950816083507</v>
       </c>
       <c r="AN6" s="3">
-        <f t="shared" si="2"/>
-        <v>11389.586779193893</v>
+        <f t="shared" si="3"/>
+        <v>10182.770324244342</v>
       </c>
       <c r="AO6" s="3">
-        <f t="shared" si="2"/>
-        <v>11503.482646985831</v>
+        <f t="shared" si="3"/>
+        <v>10284.598027486785</v>
       </c>
       <c r="AP6" s="3">
-        <f t="shared" si="2"/>
-        <v>11618.517473455689</v>
+        <f t="shared" si="3"/>
+        <v>10387.444007761653</v>
       </c>
       <c r="AQ6" s="3">
-        <f t="shared" si="2"/>
-        <v>11734.702648190247</v>
+        <f t="shared" si="3"/>
+        <v>10491.318447839269</v>
       </c>
       <c r="AR6" s="3">
-        <f t="shared" si="2"/>
-        <v>11852.049674672149</v>
+        <f t="shared" si="3"/>
+        <v>10596.231632317662</v>
       </c>
       <c r="AS6" s="3">
-        <f t="shared" si="2"/>
-        <v>11970.570171418871</v>
+        <f t="shared" si="3"/>
+        <v>10702.193948640839</v>
       </c>
       <c r="AT6" s="3">
-        <f t="shared" si="2"/>
-        <v>12090.27587313306</v>
+        <f t="shared" si="3"/>
+        <v>10809.215888127248</v>
       </c>
       <c r="AU6" s="3">
-        <f t="shared" si="2"/>
-        <v>12211.17863186439</v>
+        <f t="shared" si="3"/>
+        <v>10917.308047008521</v>
       </c>
       <c r="AV6" s="3">
-        <f t="shared" si="2"/>
-        <v>12333.290418183034</v>
+        <f t="shared" si="3"/>
+        <v>11026.481127478606</v>
       </c>
       <c r="AW6" s="3">
-        <f t="shared" si="2"/>
-        <v>12456.623322364865</v>
+        <f t="shared" si="3"/>
+        <v>11136.745938753393</v>
       </c>
       <c r="AX6" s="3">
-        <f t="shared" si="2"/>
-        <v>12581.189555588513</v>
+        <f t="shared" si="3"/>
+        <v>11248.113398140928</v>
       </c>
       <c r="AY6" s="3">
-        <f t="shared" si="2"/>
-        <v>12707.001451144399</v>
+        <f t="shared" si="3"/>
+        <v>11360.594532122337</v>
       </c>
       <c r="AZ6" s="3">
-        <f t="shared" si="2"/>
-        <v>12834.071465655843</v>
+        <f t="shared" si="3"/>
+        <v>11474.200477443561</v>
       </c>
       <c r="BA6" s="3">
-        <f t="shared" si="2"/>
-        <v>12962.412180312402</v>
+        <f t="shared" si="3"/>
+        <v>11588.942482217997</v>
       </c>
       <c r="BB6" s="3">
-        <f t="shared" si="2"/>
-        <v>13092.036302115526</v>
+        <f t="shared" si="3"/>
+        <v>11704.831907040178</v>
       </c>
       <c r="BC6" s="3">
-        <f t="shared" si="2"/>
-        <v>13222.956665136682</v>
+        <f t="shared" si="3"/>
+        <v>11821.880226110579</v>
       </c>
       <c r="BD6" s="3">
-        <f t="shared" si="2"/>
-        <v>13355.18623178805</v>
+        <f t="shared" si="3"/>
+        <v>11940.099028371686</v>
       </c>
       <c r="BE6" s="3">
-        <f t="shared" si="2"/>
-        <v>13488.738094105931</v>
+        <f t="shared" si="3"/>
+        <v>12059.500018655403</v>
       </c>
       <c r="BF6" s="3">
-        <f t="shared" si="2"/>
-        <v>13623.625475046991</v>
+        <f t="shared" si="3"/>
+        <v>12180.095018841957</v>
       </c>
       <c r="BG6" s="3">
-        <f t="shared" si="2"/>
-        <v>13759.861729797462</v>
+        <f t="shared" si="3"/>
+        <v>12301.895969030376</v>
       </c>
       <c r="BH6" s="3">
-        <f t="shared" si="2"/>
-        <v>13897.460347095437</v>
+        <f t="shared" si="3"/>
+        <v>12424.91492872068</v>
       </c>
       <c r="BI6" s="3">
-        <f t="shared" si="2"/>
-        <v>14036.434950566392</v>
+        <f t="shared" si="3"/>
+        <v>12549.164078007887</v>
       </c>
       <c r="BJ6" s="3">
-        <f t="shared" si="2"/>
-        <v>14176.799300072056</v>
+        <f t="shared" si="3"/>
+        <v>12674.655718787966</v>
       </c>
       <c r="BK6" s="3">
-        <f t="shared" si="2"/>
-        <v>14318.567293072776</v>
+        <f t="shared" si="3"/>
+        <v>12801.402275975846</v>
       </c>
       <c r="BL6" s="3">
-        <f t="shared" si="2"/>
-        <v>14461.752966003503</v>
+        <f t="shared" si="3"/>
+        <v>12929.416298735605</v>
       </c>
       <c r="BM6" s="3">
-        <f t="shared" si="2"/>
-        <v>14606.370495663539</v>
+        <f t="shared" si="3"/>
+        <v>13058.710461722962</v>
       </c>
       <c r="BN6" s="3">
-        <f t="shared" si="2"/>
-        <v>14752.434200620175</v>
+        <f t="shared" si="3"/>
+        <v>13189.297566340192</v>
       </c>
       <c r="BO6" s="3">
-        <f t="shared" si="2"/>
-        <v>14899.958542626377</v>
+        <f t="shared" si="3"/>
+        <v>13321.190542003595</v>
       </c>
       <c r="BP6" s="3">
-        <f t="shared" si="2"/>
-        <v>15048.95812805264</v>
+        <f t="shared" si="3"/>
+        <v>13454.40244742363</v>
       </c>
       <c r="BQ6" s="3">
-        <f t="shared" si="2"/>
-        <v>15199.447709333166</v>
+        <f t="shared" si="3"/>
+        <v>13588.946471897867</v>
       </c>
       <c r="BR6" s="3">
-        <f t="shared" si="2"/>
-        <v>15351.442186426499</v>
+        <f t="shared" si="3"/>
+        <v>13724.835936616846</v>
       </c>
       <c r="BS6" s="3">
-        <f t="shared" si="2"/>
-        <v>15504.956608290764</v>
+        <f t="shared" si="3"/>
+        <v>13862.084295983015</v>
       </c>
       <c r="BT6" s="3">
-        <f t="shared" si="2"/>
-        <v>15660.006174373671</v>
+        <f t="shared" si="3"/>
+        <v>14000.705138942845</v>
       </c>
       <c r="BU6" s="3">
-        <f t="shared" si="2"/>
-        <v>15816.606236117408</v>
+        <f t="shared" si="3"/>
+        <v>14140.712190332273</v>
       </c>
       <c r="BV6" s="3">
-        <f t="shared" si="2"/>
-        <v>15974.772298478581</v>
+        <f t="shared" si="3"/>
+        <v>14282.119312235596</v>
       </c>
       <c r="BW6" s="3">
-        <f t="shared" si="2"/>
-        <v>16134.520021463368</v>
+        <f t="shared" si="3"/>
+        <v>14424.940505357952</v>
       </c>
       <c r="BX6" s="3">
-        <f t="shared" si="2"/>
-        <v>16295.865221678001</v>
+        <f t="shared" si="3"/>
+        <v>14569.189910411531</v>
       </c>
       <c r="BY6" s="3">
-        <f t="shared" si="2"/>
-        <v>16458.82387389478</v>
+        <f t="shared" si="3"/>
+        <v>14714.881809515646</v>
       </c>
       <c r="BZ6" s="3">
-        <f t="shared" si="2"/>
-        <v>16623.412112633727</v>
+        <f t="shared" si="3"/>
+        <v>14862.030627610802</v>
       </c>
       <c r="CA6" s="3">
-        <f t="shared" si="2"/>
-        <v>16789.646233760064</v>
+        <f t="shared" si="3"/>
+        <v>15010.650933886911</v>
       </c>
       <c r="CB6" s="3">
-        <f t="shared" si="2"/>
-        <v>16957.542696097666</v>
+        <f t="shared" si="3"/>
+        <v>15160.757443225781</v>
       </c>
       <c r="CC6" s="3">
-        <f t="shared" si="2"/>
-        <v>17127.118123058641</v>
+        <f t="shared" si="3"/>
+        <v>15312.36501765804</v>
       </c>
       <c r="CD6" s="3">
-        <f t="shared" si="2"/>
-        <v>17298.389304289227</v>
+        <f t="shared" si="3"/>
+        <v>15465.488667834619</v>
       </c>
       <c r="CE6" s="3">
-        <f t="shared" si="2"/>
-        <v>17471.373197332119</v>
+        <f t="shared" si="3"/>
+        <v>15620.143554512966</v>
       </c>
       <c r="CF6" s="3">
-        <f t="shared" si="2"/>
-        <v>17646.086929305442</v>
+        <f t="shared" si="3"/>
+        <v>15776.344990058096</v>
       </c>
       <c r="CG6" s="3">
-        <f t="shared" si="2"/>
-        <v>17822.547798598498</v>
+        <f t="shared" si="3"/>
+        <v>15934.108439958678</v>
       </c>
       <c r="CH6" s="3">
-        <f t="shared" si="2"/>
-        <v>18000.773276584485</v>
+        <f t="shared" si="3"/>
+        <v>16093.449524358264</v>
       </c>
       <c r="CI6" s="3">
-        <f t="shared" si="2"/>
-        <v>18180.781009350329</v>
+        <f t="shared" si="3"/>
+        <v>16254.384019601846</v>
       </c>
       <c r="CJ6" s="3">
-        <f t="shared" si="2"/>
-        <v>18362.58881944383</v>
+        <f t="shared" si="3"/>
+        <v>16416.927859797866</v>
       </c>
       <c r="CK6" s="3">
-        <f t="shared" si="2"/>
-        <v>18546.214707638268</v>
+        <f t="shared" si="3"/>
+        <v>16581.097138395846</v>
       </c>
       <c r="CL6" s="3">
-        <f t="shared" si="2"/>
-        <v>18731.676854714649</v>
+        <f t="shared" si="3"/>
+        <v>16746.908109779804</v>
       </c>
       <c r="CM6" s="3">
-        <f t="shared" si="2"/>
-        <v>18918.993623261795</v>
+        <f t="shared" si="3"/>
+        <v>16914.377190877603</v>
       </c>
       <c r="CN6" s="3">
-        <f t="shared" si="2"/>
-        <v>19108.183559494413</v>
+        <f t="shared" si="3"/>
+        <v>17083.520962786381</v>
       </c>
       <c r="CO6" s="3">
-        <f t="shared" si="2"/>
-        <v>19299.265395089358</v>
+        <f t="shared" si="3"/>
+        <v>17254.356172414246</v>
       </c>
       <c r="CP6" s="3">
-        <f t="shared" si="2"/>
-        <v>19492.258049040251</v>
+        <f t="shared" si="3"/>
+        <v>17426.899734138387</v>
       </c>
       <c r="CQ6" s="3">
-        <f t="shared" si="2"/>
-        <v>19687.180629530652</v>
+        <f t="shared" si="3"/>
+        <v>17601.168731479771</v>
       </c>
       <c r="CR6" s="3">
-        <f t="shared" si="2"/>
-        <v>19884.052435825961</v>
+        <f t="shared" si="3"/>
+        <v>17777.180418794567</v>
       </c>
       <c r="CS6" s="3">
-        <f t="shared" si="2"/>
-        <v>20082.892960184221</v>
+        <f t="shared" si="3"/>
+        <v>17954.952222982512</v>
       </c>
       <c r="CT6" s="3">
-        <f t="shared" si="2"/>
-        <v>20283.721889786062</v>
+        <f t="shared" si="3"/>
+        <v>18134.501745212339</v>
       </c>
       <c r="CU6" s="3">
-        <f t="shared" ref="CU6:DC6" si="3">CT6*(1+$V$24)</f>
-        <v>20486.559108683923</v>
+        <f t="shared" ref="CU6:DC6" si="4">CT6*(1+$V$24)</f>
+        <v>18315.846762664463</v>
       </c>
       <c r="CV6" s="3">
-        <f t="shared" si="3"/>
-        <v>20691.424699770763</v>
+        <f t="shared" si="4"/>
+        <v>18499.00523029111</v>
       </c>
       <c r="CW6" s="3">
-        <f t="shared" si="3"/>
-        <v>20898.338946768472</v>
+        <f t="shared" si="4"/>
+        <v>18683.99528259402</v>
       </c>
       <c r="CX6" s="3">
-        <f t="shared" si="3"/>
-        <v>21107.322336236157</v>
+        <f t="shared" si="4"/>
+        <v>18870.83523541996</v>
       </c>
       <c r="CY6" s="3">
-        <f t="shared" si="3"/>
-        <v>21318.395559598517</v>
+        <f t="shared" si="4"/>
+        <v>19059.543587774158</v>
       </c>
       <c r="CZ6" s="3">
-        <f t="shared" si="3"/>
-        <v>21531.579515194502</v>
+        <f t="shared" si="4"/>
+        <v>19250.1390236519</v>
       </c>
       <c r="DA6" s="3">
-        <f t="shared" si="3"/>
-        <v>21746.895310346448</v>
+        <f t="shared" si="4"/>
+        <v>19442.640413888421</v>
       </c>
       <c r="DB6" s="3">
-        <f t="shared" si="3"/>
-        <v>21964.364263449912</v>
+        <f t="shared" si="4"/>
+        <v>19637.066818027306</v>
       </c>
       <c r="DC6" s="3">
-        <f t="shared" si="3"/>
-        <v>22184.007906084411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>19833.437486207578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1551,6 +1564,9 @@
       <c r="Q7" s="5">
         <v>103.319</v>
       </c>
+      <c r="R7" s="5">
+        <v>104.82899999999999</v>
+      </c>
       <c r="V7" s="3">
         <v>362.78</v>
       </c>
@@ -1565,430 +1581,434 @@
         <v>1675.1</v>
       </c>
       <c r="Z7" s="5">
-        <f>SUM(O6:U6)</f>
-        <v>2106.89</v>
+        <f>SUM(O6:R6)</f>
+        <v>2128.5389999999998</v>
       </c>
       <c r="AA7" s="3">
-        <f>Z7*(1+$X$23)</f>
-        <v>2738.9569999999999</v>
+        <f>(2555+2575)/2</f>
+        <v>2565</v>
       </c>
       <c r="AB7" s="3">
-        <f>AA7*(1+$X$23)</f>
-        <v>3560.6441</v>
+        <f t="shared" ref="AA7:AG7" si="5">AA7*(1+$X$23)</f>
+        <v>3334.5</v>
       </c>
       <c r="AC7" s="3">
-        <f>AB7*(1+$X$23)</f>
-        <v>4628.8373300000003</v>
+        <f t="shared" si="5"/>
+        <v>4334.8500000000004</v>
       </c>
       <c r="AD7" s="3">
-        <f>AC7*(1+$X$23)</f>
-        <v>6017.4885290000002</v>
+        <f t="shared" si="5"/>
+        <v>5635.3050000000003</v>
       </c>
       <c r="AE7" s="3">
-        <f>AD7*(1+$X$23)</f>
-        <v>7822.7350877000008</v>
+        <f t="shared" si="5"/>
+        <v>7325.8965000000007</v>
       </c>
       <c r="AF7" s="3">
-        <f>AE7*(1+$X$23)</f>
-        <v>10169.555614010002</v>
+        <f t="shared" si="5"/>
+        <v>9523.6654500000004</v>
       </c>
       <c r="AG7" s="3">
-        <f>AF7*(1+$X$23)</f>
-        <v>13220.422298213003</v>
+        <f t="shared" si="5"/>
+        <v>12380.765085000001</v>
       </c>
       <c r="AH7" s="3">
         <f>AG7*(1+$V$24)</f>
-        <v>13352.626521195134</v>
+        <v>12504.572735850001</v>
       </c>
       <c r="AI7" s="3">
         <f>AH7*(1+$V$24)</f>
-        <v>13486.152786407085</v>
+        <v>12629.618463208501</v>
       </c>
       <c r="AJ7" s="3">
-        <f t="shared" ref="AJ7:CU7" si="4">AI7*(1+$V$24)</f>
-        <v>13621.014314271157</v>
+        <f t="shared" ref="AJ7:CU7" si="6">AI7*(1+$V$24)</f>
+        <v>12755.914647840586</v>
       </c>
       <c r="AK7" s="3">
-        <f t="shared" si="4"/>
-        <v>13757.224457413868</v>
+        <f t="shared" si="6"/>
+        <v>12883.473794318992</v>
       </c>
       <c r="AL7" s="3">
-        <f t="shared" si="4"/>
-        <v>13894.796701988007</v>
+        <f t="shared" si="6"/>
+        <v>13012.308532262183</v>
       </c>
       <c r="AM7" s="3">
-        <f t="shared" si="4"/>
-        <v>14033.744669007887</v>
+        <f t="shared" si="6"/>
+        <v>13142.431617584805</v>
       </c>
       <c r="AN7" s="3">
-        <f t="shared" si="4"/>
-        <v>14174.082115697965</v>
+        <f t="shared" si="6"/>
+        <v>13273.855933760653</v>
       </c>
       <c r="AO7" s="3">
-        <f t="shared" si="4"/>
-        <v>14315.822936854946</v>
+        <f t="shared" si="6"/>
+        <v>13406.594493098261</v>
       </c>
       <c r="AP7" s="3">
-        <f t="shared" si="4"/>
-        <v>14458.981166223495</v>
+        <f t="shared" si="6"/>
+        <v>13540.660438029243</v>
       </c>
       <c r="AQ7" s="3">
-        <f t="shared" si="4"/>
-        <v>14603.570977885731</v>
+        <f t="shared" si="6"/>
+        <v>13676.067042409535</v>
       </c>
       <c r="AR7" s="3">
-        <f t="shared" si="4"/>
-        <v>14749.606687664589</v>
+        <f t="shared" si="6"/>
+        <v>13812.82771283363</v>
       </c>
       <c r="AS7" s="3">
-        <f t="shared" si="4"/>
-        <v>14897.102754541234</v>
+        <f t="shared" si="6"/>
+        <v>13950.955989961967</v>
       </c>
       <c r="AT7" s="3">
-        <f t="shared" si="4"/>
-        <v>15046.073782086647</v>
+        <f t="shared" si="6"/>
+        <v>14090.465549861587</v>
       </c>
       <c r="AU7" s="3">
-        <f t="shared" si="4"/>
-        <v>15196.534519907515</v>
+        <f t="shared" si="6"/>
+        <v>14231.370205360203</v>
       </c>
       <c r="AV7" s="3">
-        <f t="shared" si="4"/>
-        <v>15348.499865106591</v>
+        <f t="shared" si="6"/>
+        <v>14373.683907413804</v>
       </c>
       <c r="AW7" s="3">
-        <f t="shared" si="4"/>
-        <v>15501.984863757656</v>
+        <f t="shared" si="6"/>
+        <v>14517.420746487942</v>
       </c>
       <c r="AX7" s="3">
-        <f t="shared" si="4"/>
-        <v>15657.004712395234</v>
+        <f t="shared" si="6"/>
+        <v>14662.594953952821</v>
       </c>
       <c r="AY7" s="3">
-        <f t="shared" si="4"/>
-        <v>15813.574759519186</v>
+        <f t="shared" si="6"/>
+        <v>14809.220903492349</v>
       </c>
       <c r="AZ7" s="3">
-        <f t="shared" si="4"/>
-        <v>15971.710507114378</v>
+        <f t="shared" si="6"/>
+        <v>14957.313112527272</v>
       </c>
       <c r="BA7" s="3">
-        <f t="shared" si="4"/>
-        <v>16131.427612185522</v>
+        <f t="shared" si="6"/>
+        <v>15106.886243652545</v>
       </c>
       <c r="BB7" s="3">
-        <f t="shared" si="4"/>
-        <v>16292.741888307377</v>
+        <f t="shared" si="6"/>
+        <v>15257.95510608907</v>
       </c>
       <c r="BC7" s="3">
-        <f t="shared" si="4"/>
-        <v>16455.669307190452</v>
+        <f t="shared" si="6"/>
+        <v>15410.534657149961</v>
       </c>
       <c r="BD7" s="3">
-        <f t="shared" si="4"/>
-        <v>16620.226000262355</v>
+        <f t="shared" si="6"/>
+        <v>15564.640003721461</v>
       </c>
       <c r="BE7" s="3">
-        <f t="shared" si="4"/>
-        <v>16786.42826026498</v>
+        <f t="shared" si="6"/>
+        <v>15720.286403758675</v>
       </c>
       <c r="BF7" s="3">
-        <f t="shared" si="4"/>
-        <v>16954.292542867632</v>
+        <f t="shared" si="6"/>
+        <v>15877.489267796262</v>
       </c>
       <c r="BG7" s="3">
-        <f t="shared" si="4"/>
-        <v>17123.835468296307</v>
+        <f t="shared" si="6"/>
+        <v>16036.264160474224</v>
       </c>
       <c r="BH7" s="3">
-        <f t="shared" si="4"/>
-        <v>17295.07382297927</v>
+        <f t="shared" si="6"/>
+        <v>16196.626802078967</v>
       </c>
       <c r="BI7" s="3">
-        <f t="shared" si="4"/>
-        <v>17468.024561209062</v>
+        <f t="shared" si="6"/>
+        <v>16358.593070099756</v>
       </c>
       <c r="BJ7" s="3">
-        <f t="shared" si="4"/>
-        <v>17642.704806821152</v>
+        <f t="shared" si="6"/>
+        <v>16522.179000800752</v>
       </c>
       <c r="BK7" s="3">
-        <f t="shared" si="4"/>
-        <v>17819.131854889365</v>
+        <f t="shared" si="6"/>
+        <v>16687.400790808759</v>
       </c>
       <c r="BL7" s="3">
-        <f t="shared" si="4"/>
-        <v>17997.323173438257</v>
+        <f t="shared" si="6"/>
+        <v>16854.274798716848</v>
       </c>
       <c r="BM7" s="3">
-        <f t="shared" si="4"/>
-        <v>18177.296405172641</v>
+        <f t="shared" si="6"/>
+        <v>17022.817546704016</v>
       </c>
       <c r="BN7" s="3">
-        <f t="shared" si="4"/>
-        <v>18359.069369224369</v>
+        <f t="shared" si="6"/>
+        <v>17193.045722171057</v>
       </c>
       <c r="BO7" s="3">
-        <f t="shared" si="4"/>
-        <v>18542.660062916613</v>
+        <f t="shared" si="6"/>
+        <v>17364.976179392768</v>
       </c>
       <c r="BP7" s="3">
-        <f t="shared" si="4"/>
-        <v>18728.086663545779</v>
+        <f t="shared" si="6"/>
+        <v>17538.625941186696</v>
       </c>
       <c r="BQ7" s="3">
-        <f t="shared" si="4"/>
-        <v>18915.367530181236</v>
+        <f t="shared" si="6"/>
+        <v>17714.012200598561</v>
       </c>
       <c r="BR7" s="3">
-        <f t="shared" si="4"/>
-        <v>19104.521205483048</v>
+        <f t="shared" si="6"/>
+        <v>17891.152322604546</v>
       </c>
       <c r="BS7" s="3">
-        <f t="shared" si="4"/>
-        <v>19295.566417537877</v>
+        <f t="shared" si="6"/>
+        <v>18070.063845830591</v>
       </c>
       <c r="BT7" s="3">
-        <f t="shared" si="4"/>
-        <v>19488.522081713258</v>
+        <f t="shared" si="6"/>
+        <v>18250.764484288899</v>
       </c>
       <c r="BU7" s="3">
-        <f t="shared" si="4"/>
-        <v>19683.407302530391</v>
+        <f t="shared" si="6"/>
+        <v>18433.272129131787</v>
       </c>
       <c r="BV7" s="3">
-        <f t="shared" si="4"/>
-        <v>19880.241375555695</v>
+        <f t="shared" si="6"/>
+        <v>18617.604850423104</v>
       </c>
       <c r="BW7" s="3">
-        <f t="shared" si="4"/>
-        <v>20079.043789311254</v>
+        <f t="shared" si="6"/>
+        <v>18803.780898927336</v>
       </c>
       <c r="BX7" s="3">
-        <f t="shared" si="4"/>
-        <v>20279.834227204366</v>
+        <f t="shared" si="6"/>
+        <v>18991.818707916609</v>
       </c>
       <c r="BY7" s="3">
-        <f t="shared" si="4"/>
-        <v>20482.632569476409</v>
+        <f t="shared" si="6"/>
+        <v>19181.736894995774</v>
       </c>
       <c r="BZ7" s="3">
-        <f t="shared" si="4"/>
-        <v>20687.458895171174</v>
+        <f t="shared" si="6"/>
+        <v>19373.554263945731</v>
       </c>
       <c r="CA7" s="3">
-        <f t="shared" si="4"/>
-        <v>20894.333484122886</v>
+        <f t="shared" si="6"/>
+        <v>19567.289806585188</v>
       </c>
       <c r="CB7" s="3">
-        <f t="shared" si="4"/>
-        <v>21103.276818964114</v>
+        <f t="shared" si="6"/>
+        <v>19762.96270465104</v>
       </c>
       <c r="CC7" s="3">
-        <f t="shared" si="4"/>
-        <v>21314.309587153755</v>
+        <f t="shared" si="6"/>
+        <v>19960.59233169755</v>
       </c>
       <c r="CD7" s="3">
-        <f t="shared" si="4"/>
-        <v>21527.452683025294</v>
+        <f t="shared" si="6"/>
+        <v>20160.198255014526</v>
       </c>
       <c r="CE7" s="3">
-        <f t="shared" si="4"/>
-        <v>21742.727209855548</v>
+        <f t="shared" si="6"/>
+        <v>20361.800237564672</v>
       </c>
       <c r="CF7" s="3">
-        <f t="shared" si="4"/>
-        <v>21960.154481954105</v>
+        <f t="shared" si="6"/>
+        <v>20565.418239940318</v>
       </c>
       <c r="CG7" s="3">
-        <f t="shared" si="4"/>
-        <v>22179.756026773648</v>
+        <f t="shared" si="6"/>
+        <v>20771.072422339723</v>
       </c>
       <c r="CH7" s="3">
-        <f t="shared" si="4"/>
-        <v>22401.553587041384</v>
+        <f t="shared" si="6"/>
+        <v>20978.783146563121</v>
       </c>
       <c r="CI7" s="3">
-        <f t="shared" si="4"/>
-        <v>22625.569122911798</v>
+        <f t="shared" si="6"/>
+        <v>21188.570978028751</v>
       </c>
       <c r="CJ7" s="3">
-        <f t="shared" si="4"/>
-        <v>22851.824814140917</v>
+        <f t="shared" si="6"/>
+        <v>21400.456687809037</v>
       </c>
       <c r="CK7" s="3">
-        <f t="shared" si="4"/>
-        <v>23080.343062282325</v>
+        <f t="shared" si="6"/>
+        <v>21614.461254687129</v>
       </c>
       <c r="CL7" s="3">
-        <f t="shared" si="4"/>
-        <v>23311.146492905147</v>
+        <f t="shared" si="6"/>
+        <v>21830.605867234</v>
       </c>
       <c r="CM7" s="3">
-        <f t="shared" si="4"/>
-        <v>23544.257957834197</v>
+        <f t="shared" si="6"/>
+        <v>22048.911925906341</v>
       </c>
       <c r="CN7" s="3">
-        <f t="shared" si="4"/>
-        <v>23779.70053741254</v>
+        <f t="shared" si="6"/>
+        <v>22269.401045165403</v>
       </c>
       <c r="CO7" s="3">
-        <f t="shared" si="4"/>
-        <v>24017.497542786667</v>
+        <f t="shared" si="6"/>
+        <v>22492.095055617057</v>
       </c>
       <c r="CP7" s="3">
-        <f t="shared" si="4"/>
-        <v>24257.672518214535</v>
+        <f t="shared" si="6"/>
+        <v>22717.016006173228</v>
       </c>
       <c r="CQ7" s="3">
-        <f t="shared" si="4"/>
-        <v>24500.24924339668</v>
+        <f t="shared" si="6"/>
+        <v>22944.186166234958</v>
       </c>
       <c r="CR7" s="3">
-        <f t="shared" si="4"/>
-        <v>24745.251735830647</v>
+        <f t="shared" si="6"/>
+        <v>23173.62802789731</v>
       </c>
       <c r="CS7" s="3">
-        <f t="shared" si="4"/>
-        <v>24992.704253188953</v>
+        <f t="shared" si="6"/>
+        <v>23405.364308176282</v>
       </c>
       <c r="CT7" s="3">
-        <f t="shared" si="4"/>
-        <v>25242.631295720843</v>
+        <f t="shared" si="6"/>
+        <v>23639.417951258045</v>
       </c>
       <c r="CU7" s="3">
-        <f t="shared" si="4"/>
-        <v>25495.057608678053</v>
+        <f t="shared" si="6"/>
+        <v>23875.812130770624</v>
       </c>
       <c r="CV7" s="3">
-        <f t="shared" ref="CV7:DC7" si="5">CU7*(1+$V$24)</f>
-        <v>25750.008184764833</v>
+        <f t="shared" ref="CV7:DC7" si="7">CU7*(1+$V$24)</f>
+        <v>24114.570252078331</v>
       </c>
       <c r="CW7" s="3">
-        <f t="shared" si="5"/>
-        <v>26007.50826661248</v>
+        <f t="shared" si="7"/>
+        <v>24355.715954599113</v>
       </c>
       <c r="CX7" s="3">
-        <f t="shared" si="5"/>
-        <v>26267.583349278604</v>
+        <f t="shared" si="7"/>
+        <v>24599.273114145104</v>
       </c>
       <c r="CY7" s="3">
-        <f t="shared" si="5"/>
-        <v>26530.259182771391</v>
+        <f t="shared" si="7"/>
+        <v>24845.265845286554</v>
       </c>
       <c r="CZ7" s="3">
-        <f t="shared" si="5"/>
-        <v>26795.561774599104</v>
+        <f t="shared" si="7"/>
+        <v>25093.718503739419</v>
       </c>
       <c r="DA7" s="3">
-        <f t="shared" si="5"/>
-        <v>27063.517392345097</v>
+        <f t="shared" si="7"/>
+        <v>25344.655688776813</v>
       </c>
       <c r="DB7" s="3">
-        <f t="shared" si="5"/>
-        <v>27334.152566268549</v>
+        <f t="shared" si="7"/>
+        <v>25598.102245664581</v>
       </c>
       <c r="DC7" s="3">
-        <f t="shared" si="5"/>
-        <v>27607.494091931236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>25854.083268121227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
-        <f t="shared" ref="E8:Q8" si="6">+E6-E7</f>
+        <f t="shared" ref="E8:R8" si="8">+E6-E7</f>
         <v>120.691</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>136.67500000000001</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>151.88300000000001</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>176.45100000000002</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>207.15600000000001</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>259.04899999999998</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>288.56799999999998</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>324.21299999999997</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>342.93400000000003</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>372.642</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>381.8</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>407.79399999999998</v>
       </c>
       <c r="Q8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>444.21699999999993</v>
       </c>
+      <c r="R8" s="6">
+        <f t="shared" si="8"/>
+        <v>484.82</v>
+      </c>
       <c r="Z8" s="24">
-        <f>(Z7-Y7)/Y7</f>
-        <v>0.25776968539191691</v>
+        <f t="shared" ref="Z8:AH8" si="9">(Z7-Y7)/Y7</f>
+        <v>0.27069368992895937</v>
       </c>
       <c r="AA8" s="22">
-        <f>(AA7-Z7)/Z7</f>
+        <f t="shared" si="9"/>
+        <v>0.20505191589160465</v>
+      </c>
+      <c r="AB8" s="22">
+        <f t="shared" si="9"/>
+        <v>0.3</v>
+      </c>
+      <c r="AC8" s="22">
+        <f t="shared" si="9"/>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="AD8" s="22">
+        <f t="shared" si="9"/>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="AE8" s="22">
+        <f t="shared" si="9"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="AB8" s="22">
-        <f>(AB7-AA7)/AA7</f>
+      <c r="AF8" s="22">
+        <f t="shared" si="9"/>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="AG8" s="22">
+        <f t="shared" si="9"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="AC8" s="22">
-        <f>(AC7-AB7)/AB7</f>
-        <v>0.3000000000000001</v>
-      </c>
-      <c r="AD8" s="22">
-        <f>(AD7-AC7)/AC7</f>
-        <v>0.29999999999999993</v>
-      </c>
-      <c r="AE8" s="22">
-        <f>(AE7-AD7)/AD7</f>
-        <v>0.3000000000000001</v>
-      </c>
-      <c r="AF8" s="22">
-        <f>(AF7-AE7)/AE7</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="AG8" s="22">
-        <f>(AG7-AF7)/AF7</f>
-        <v>0.3000000000000001</v>
-      </c>
       <c r="AH8" s="22">
-        <f>(AH7-AG7)/AG7</f>
-        <v>1.0000000000000064E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>9.9999999999999863E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -2033,8 +2053,11 @@
       <c r="Q9" s="5">
         <v>240.22499999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R9" s="5">
+        <v>253.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2079,8 +2102,11 @@
       <c r="Q10" s="5">
         <v>156.87</v>
       </c>
-    </row>
-    <row r="11" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R10" s="5">
+        <v>159.97999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
@@ -2125,98 +2151,105 @@
       <c r="Q11" s="5">
         <v>51.351999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R11" s="5">
+        <v>43.847999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
-        <f t="shared" ref="E12:Q12" si="7">SUM(E9:E11)</f>
+        <f t="shared" ref="E12:R12" si="10">SUM(E9:E11)</f>
         <v>129.958</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>145.613</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>164.71299999999999</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>186.33699999999999</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>212.05100000000002</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>250.59399999999999</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>278.154</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>327.35199999999998</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>374.27599999999995</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>407.27</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>416.77</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>429.62</v>
       </c>
       <c r="Q12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>448.447</v>
       </c>
-    </row>
-    <row r="13" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R12" s="6">
+        <f t="shared" si="10"/>
+        <v>457.07800000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
-        <f t="shared" ref="E13:Q13" si="8">E8-E12</f>
+        <f t="shared" ref="E13:R13" si="11">E8-E12</f>
         <v>-9.2669999999999959</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-8.9379999999999882</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-12.829999999999984</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-9.8859999999999673</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-4.8950000000000102</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>8.4549999999999841</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>10.413999999999987</v>
       </c>
       <c r="L13" s="6">
@@ -2224,27 +2257,31 @@
         <v>-3.13900000000001</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-31.341999999999928</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-34.627999999999986</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-34.96999999999997</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-21.826000000000022</v>
       </c>
       <c r="Q13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-4.230000000000075</v>
       </c>
-    </row>
-    <row r="14" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R13" s="6">
+        <f t="shared" si="11"/>
+        <v>27.741999999999962</v>
+      </c>
+    </row>
+    <row r="14" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
@@ -2299,67 +2336,75 @@
         <f>-1.303+29.883</f>
         <v>28.58</v>
       </c>
-    </row>
-    <row r="15" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R14" s="5">
+        <f>-1.292+30.817</f>
+        <v>29.524999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
-        <f t="shared" ref="E15:Q15" si="9">+E13+E14</f>
+        <f t="shared" ref="E15:R15" si="12">+E13+E14</f>
         <v>-14.554999999999996</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-15.166999999999987</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-12.528999999999986</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-9.6579999999999675</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-4.7670000000000101</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8.531999999999984</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10.853999999999989</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-1.1000000000010779E-2</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-22.21599999999993</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-25.009999999999987</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-20.423999999999971</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.72800000000002285</v>
       </c>
       <c r="Q15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>24.349999999999923</v>
       </c>
-    </row>
-    <row r="16" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R15" s="6">
+        <f t="shared" si="12"/>
+        <v>57.26699999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:107" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
@@ -2404,126 +2449,137 @@
       <c r="Q16" s="5">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R16" s="5">
+        <v>3.274</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
-        <f t="shared" ref="E17:Q17" si="10">+E15-E16</f>
+        <f t="shared" ref="E17:R17" si="13">+E15-E16</f>
         <v>-15.149999999999997</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-16.159999999999986</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-11.989999999999986</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-6.6979999999999675</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.0500000000000105</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.1689999999999845</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9.7379999999999889</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.8790000000000111</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-25.141999999999932</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-28.189999999999987</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-24.08599999999997</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-3.7890000000000228</v>
       </c>
       <c r="Q17" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22.679999999999922</v>
       </c>
-    </row>
-    <row r="18" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R17" s="6">
+        <f t="shared" si="13"/>
+        <v>53.992999999999959</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7">
-        <f t="shared" ref="E18:Q18" si="11">+E17/E19</f>
+        <f t="shared" ref="E18:R18" si="14">+E17/E19</f>
         <v>-5.0073705850856368E-2</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-5.3147929500060795E-2</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-3.9178653352241861E-2</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-2.1745411809011676E-2</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-1.3054114947122809E-2</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2.0727021455604115E-2</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2.8171540321927365E-2</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-1.5498975523753589E-2</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-7.9565809044589805E-2</v>
       </c>
       <c r="N18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-8.8829928028536453E-2</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-7.5437068960117162E-2</v>
       </c>
       <c r="P18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-1.1759229086169245E-2</v>
       </c>
       <c r="Q18" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>6.9665219915406279E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R18" s="7">
+        <f t="shared" si="14"/>
+        <v>0.16416485504492304</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
@@ -2568,8 +2624,11 @@
       <c r="Q19" s="5">
         <v>325.55700000000002</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R19" s="5">
+        <v>328.89499999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
@@ -2580,76 +2639,80 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10">
-        <f t="shared" ref="I21:K21" si="12">+I6/E6-1</f>
+        <f t="shared" ref="I21:K21" si="15">+I6/E6-1</f>
         <v>0.74875060610958455</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.83741431074009598</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.82841515192723181</v>
       </c>
       <c r="L21" s="10">
-        <f>+L6/H6-1</f>
+        <f t="shared" ref="L21:S21" si="16">+L6/H6-1</f>
         <v>0.73898411040081502</v>
       </c>
       <c r="M21" s="10">
-        <f>+M6/I6-1</f>
+        <f t="shared" si="16"/>
         <v>0.61387196474520134</v>
       </c>
       <c r="N21" s="10">
-        <f>+N6/J6-1</f>
+        <f t="shared" si="16"/>
         <v>0.43900023911857233</v>
       </c>
       <c r="O21" s="10">
-        <f>+O6/K6-1</f>
+        <f t="shared" si="16"/>
         <v>0.32692614935404807</v>
       </c>
       <c r="P21" s="10">
-        <f>+P6/L6-1</f>
+        <f t="shared" si="16"/>
         <v>0.25484441249033574</v>
       </c>
       <c r="Q21" s="10">
-        <f>+Q6/M6-1</f>
+        <f t="shared" si="16"/>
         <v>0.25428318134024219</v>
       </c>
       <c r="R21" s="10">
-        <f>+R6/N6-1</f>
-        <v>0.21005796774172936</v>
-      </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
+        <f t="shared" si="16"/>
+        <v>0.25617864545940661</v>
+      </c>
+      <c r="S21" s="10">
+        <f t="shared" si="16"/>
+        <v>0.22271721394852539</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E22" s="12">
-        <f t="shared" ref="E22:H22" si="13">+E8/E6</f>
+        <f t="shared" ref="E22:H22" si="17">+E8/E6</f>
         <v>0.78028770001616288</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.76986554460911061</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.7649648197674126</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.75552025485015994</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:K22" si="14">+I8/I6</f>
+        <f t="shared" ref="I22:K22" si="18">+I8/I6</f>
         <v>0.76586022300434775</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.79414649997854059</v>
       </c>
       <c r="K22" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.79488747486433631</v>
       </c>
       <c r="L22" s="12">
@@ -2657,24 +2720,28 @@
         <v>0.79828284967178642</v>
       </c>
       <c r="M22" s="12">
-        <f t="shared" ref="M22:Q22" si="15">+M8/M6</f>
+        <f t="shared" ref="M22:R22" si="19">+M8/M6</f>
         <v>0.78558551129009724</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.79387045988593929</v>
       </c>
       <c r="O22" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.79258647247121738</v>
       </c>
       <c r="P22" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.8001608978887057</v>
       </c>
       <c r="Q22" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.81130190526285029</v>
+      </c>
+      <c r="R22" s="12">
+        <f t="shared" si="19"/>
+        <v>0.82221796356815668</v>
       </c>
       <c r="U22" t="s">
         <v>71</v>
@@ -2686,12 +2753,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="U23" s="15" t="s">
         <v>62</v>
       </c>
       <c r="V23" s="23">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="W23" s="15" t="s">
         <v>62</v>
@@ -2700,7 +2767,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
@@ -2729,7 +2796,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
@@ -2756,7 +2823,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
@@ -2783,17 +2850,17 @@
       </c>
       <c r="V26" s="18">
         <f>NPV(V25,V6:DC6)</f>
-        <v>58324.781680299697</v>
+        <v>53169.98322190965</v>
       </c>
       <c r="W26" s="17" t="s">
         <v>63</v>
       </c>
       <c r="X26" s="26">
         <f>NPV($V$25,V7:DC7)</f>
-        <v>70118.732659662914</v>
-      </c>
-    </row>
-    <row r="27" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>65936.250330536161</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
@@ -2818,17 +2885,17 @@
       </c>
       <c r="V27" s="21">
         <f>Main!$O$3</f>
-        <v>325.55700000000002</v>
+        <v>328</v>
       </c>
       <c r="W27" s="17" t="s">
         <v>1</v>
       </c>
       <c r="X27" s="21">
         <f>Main!$O$3</f>
-        <v>325.55700000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
@@ -2853,17 +2920,17 @@
       </c>
       <c r="V28" s="19">
         <f>V26/V27</f>
-        <v>179.1538246153506</v>
+        <v>162.10360738387089</v>
       </c>
       <c r="W28" s="17" t="s">
         <v>64</v>
       </c>
       <c r="X28" s="19">
         <f>X26/X27</f>
-        <v>215.38081706018579</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>201.02515344675658</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>37</v>
       </c>
@@ -2888,17 +2955,17 @@
       </c>
       <c r="V29" s="20">
         <f>(V28-Main!$O$2)/Main!$O$2</f>
-        <v>0.32795066796642652</v>
+        <v>0.24944972548073749</v>
       </c>
       <c r="W29" s="17" t="s">
         <v>65</v>
       </c>
       <c r="X29" s="20">
         <f>(X28-Main!$O$2)/Main!$O$2</f>
-        <v>0.59647777822389592</v>
-      </c>
-    </row>
-    <row r="30" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.549446226659138</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>38</v>
       </c>
@@ -2925,17 +2992,17 @@
       </c>
       <c r="V30" s="18">
         <f>V27*V28</f>
-        <v>58324.781680299697</v>
+        <v>53169.983221909657</v>
       </c>
       <c r="W30" s="17" t="s">
         <v>66</v>
       </c>
       <c r="X30" s="18">
         <f>X27*X28</f>
-        <v>70118.732659662914</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>65936.250330536161</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2956,7 +3023,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -2979,7 +3046,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="34" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>40</v>
       </c>
@@ -3000,7 +3067,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>41</v>
       </c>
@@ -3021,7 +3088,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>37</v>
       </c>
@@ -3044,7 +3111,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>42</v>
       </c>
@@ -3067,7 +3134,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>4</v>
       </c>
@@ -3088,7 +3155,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
@@ -3109,7 +3176,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>43</v>
       </c>
@@ -3130,7 +3197,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>44</v>
       </c>
@@ -3153,7 +3220,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="43" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>48</v>
       </c>
@@ -3173,7 +3240,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
     </row>
-    <row r="44" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>49</v>
       </c>
@@ -3192,7 +3259,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>50</v>
       </c>
@@ -3211,7 +3278,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
     </row>
-    <row r="46" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>51</v>
       </c>
@@ -3230,7 +3297,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
     </row>
-    <row r="47" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>52</v>
       </c>
@@ -3249,7 +3316,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
     </row>
-    <row r="48" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>53</v>
       </c>
@@ -3268,7 +3335,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>54</v>
       </c>
@@ -3287,7 +3354,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
     </row>
-    <row r="50" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>37</v>
       </c>
@@ -3306,7 +3373,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
     </row>
-    <row r="51" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>33</v>
       </c>
@@ -3325,7 +3392,7 @@
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
     </row>
-    <row r="52" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>55</v>
       </c>
@@ -3344,7 +3411,7 @@
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
     </row>
-    <row r="53" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>56</v>
       </c>
@@ -3364,7 +3431,7 @@
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
     </row>
-    <row r="54" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>57</v>
       </c>

</xml_diff>